<commit_message>
mé g e g y picikécske excelecsecske
</commit_message>
<xml_diff>
--- a/documentation/Test Documents/Program_Test.xlsx
+++ b/documentation/Test Documents/Program_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
   <si>
     <t>Sorszám</t>
   </si>
@@ -66,15 +66,6 @@
     <t>Terület=314,16 Kerület=62,83</t>
   </si>
   <si>
-    <t>a oldal=10 e átló=10 f átló=17,3</t>
-  </si>
-  <si>
-    <t>Terület=86 Kerület=40</t>
-  </si>
-  <si>
-    <t>Terület=86,50 Kerület=40</t>
-  </si>
-  <si>
     <t>a oldal=10 b oldal=10</t>
   </si>
   <si>
@@ -277,6 +268,69 @@
   </si>
   <si>
     <t>Kör érvénytelen adatok megadása</t>
+  </si>
+  <si>
+    <t>Deltoid érvénytelen adatok megadása</t>
+  </si>
+  <si>
+    <t>a oldal=, b oldal=, f étló=- e átló=-</t>
+  </si>
+  <si>
+    <t>a oldal=0 b oldal=0 f étló=0 e átló=0</t>
+  </si>
+  <si>
+    <t>Terület=491511175694552000000000,00 Kerület=3965899345952,40</t>
+  </si>
+  <si>
+    <t>a oldal=4,4 b oldal=4,4 f étló=4,4 e átló=4,4</t>
+  </si>
+  <si>
+    <t>Terület=9,68 Kerület=17,60</t>
+  </si>
+  <si>
+    <t>Terület=9.680000000000001 Kerület=17.6</t>
+  </si>
+  <si>
+    <t>Terület=4.915111756945523e+23 cm^2 Kerület=3965899345952.4</t>
+  </si>
+  <si>
+    <t>a oldal=10 e átló=10 f átló=17,5</t>
+  </si>
+  <si>
+    <t>Terület=86 Kerület=42</t>
+  </si>
+  <si>
+    <t>Terület=86,50 Kerület=42</t>
+  </si>
+  <si>
+    <t>a oldal=10 e átló=10 f átló=17,6</t>
+  </si>
+  <si>
+    <t>Terület=86 Kerület=43</t>
+  </si>
+  <si>
+    <t>Terület=86,50 Kerület=43</t>
+  </si>
+  <si>
+    <t>a oldal=10 e átló=10 f átló=17,7</t>
+  </si>
+  <si>
+    <t>Terület=86 Kerület=44</t>
+  </si>
+  <si>
+    <t>Terület=86,50 Kerület=44</t>
+  </si>
+  <si>
+    <t>a oldal=, e átló=- f átló=-</t>
+  </si>
+  <si>
+    <t>a oldal=0 e átló=0 f átló=0</t>
+  </si>
+  <si>
+    <t>Rombusz érvénytelen adatok megadása</t>
+  </si>
+  <si>
+    <t>a oldal=991474836488,1 b oldal=991474836488,1 f étló=991474836488,1 e átló=991474836488,1</t>
   </si>
 </sst>
 </file>
@@ -597,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,12 +668,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -644,16 +698,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -661,16 +715,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -679,10 +733,10 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -697,16 +751,16 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -715,16 +769,16 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -736,16 +790,16 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -754,16 +808,16 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -772,7 +826,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -790,16 +844,16 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -808,16 +862,16 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -829,16 +883,16 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -847,16 +901,16 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -865,7 +919,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -883,16 +937,16 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -901,16 +955,16 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -922,16 +976,16 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -940,16 +994,16 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -958,16 +1012,16 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -976,13 +1030,13 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -994,16 +1048,16 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -1015,16 +1069,16 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -1033,16 +1087,16 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
@@ -1051,16 +1105,16 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -1069,7 +1123,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -1087,16 +1141,16 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -1108,16 +1162,16 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -1126,16 +1180,16 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s">
         <v>6</v>
@@ -1144,16 +1198,16 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -1162,16 +1216,16 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -1180,16 +1234,16 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -1197,42 +1251,170 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>